<commit_message>
v2.0 Fix push buttons
</commit_message>
<xml_diff>
--- a/GPSLCD_Parts_List.xlsx
+++ b/GPSLCD_Parts_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27805"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -107,13 +107,13 @@
     <t>Enclosure</t>
   </si>
   <si>
-    <t>Computer City</t>
-  </si>
-  <si>
     <t>SS12D00G4 SPDT 1P2T 2 Position 3 Pin PCB Panel Vertical Slide Switch</t>
   </si>
   <si>
     <t>http://www.ebay.com/itm/20-pcs-SS12D00G4-SPDT-1P2T-2-Position-3-Pin-PCB-Panel-Vertical-Slide-Switch-/401230840373?hash=item5d6b38c235:g:zAUAAOSw4GVYNT-6</t>
+  </si>
+  <si>
+    <t>Micro Center</t>
   </si>
 </sst>
 </file>
@@ -615,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,10 +730,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="49" thickBot="1" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
v2.0 Fix push buttob
</commit_message>
<xml_diff>
--- a/GPSLCD_Parts_List.xlsx
+++ b/GPSLCD_Parts_List.xlsx
@@ -86,9 +86,6 @@
     <t>OFF-(ON) N/O Push-Button Switch</t>
   </si>
   <si>
-    <t>http://www.ebay.com/itm/171854289731?_trksid=p2055119.m1438.l2649&amp;ssPageName=STRK%3AMEBIDX%3AIT</t>
-  </si>
-  <si>
     <t>10K Ohm resistors</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Micro Center</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/10-Pcs-AC-125V-3A-250V-1-5A-SPST-On-Off-Latching-Red-Push-Button-Switch-/321195563845?hash=item4ac8bf5b45:g:rToAAOSwn7JYDood</t>
   </si>
 </sst>
 </file>
@@ -615,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,13 +730,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -744,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="81" thickBot="1" x14ac:dyDescent="0.25">
@@ -752,21 +752,21 @@
         <v>7</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="14" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -774,10 +774,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>